<commit_message>
step 5 in progress
</commit_message>
<xml_diff>
--- a/bot_outputs/step_3_out.xlsx
+++ b/bot_outputs/step_3_out.xlsx
@@ -70,7 +70,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -80,7 +80,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13136,7 +13135,7 @@
       <c r="B2" s="8" t="n">
         <v>52.61</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="8" t="n">
         <v>3.93</v>
       </c>
     </row>
@@ -13147,7 +13146,7 @@
       <c r="B3" s="8" t="n">
         <v>53.46</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="8" t="n">
         <v>3.391</v>
       </c>
     </row>
@@ -13158,7 +13157,7 @@
       <c r="B4" s="8" t="n">
         <v>49.67</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="8" t="n">
         <v>2.627</v>
       </c>
     </row>
@@ -13169,7 +13168,7 @@
       <c r="B5" s="8" t="n">
         <v>51.12</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="8" t="n">
         <v>3.175</v>
       </c>
     </row>
@@ -13180,7 +13179,7 @@
       <c r="B6" s="8" t="n">
         <v>48.54</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="8" t="n">
         <v>3.142</v>
       </c>
     </row>
@@ -13191,7 +13190,7 @@
       <c r="B7" s="8" t="n">
         <v>45.2</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="8" t="n">
         <v>3.236</v>
       </c>
     </row>
@@ -13202,7 +13201,7 @@
       <c r="B8" s="8" t="n">
         <v>46.68</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="8" t="n">
         <v>3.067</v>
       </c>
     </row>
@@ -13213,7 +13212,7 @@
       <c r="B9" s="8" t="n">
         <v>48.06</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="8" t="n">
         <v>2.969</v>
       </c>
     </row>
@@ -13224,7 +13223,7 @@
       <c r="B10" s="8" t="n">
         <v>49.88</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="8" t="n">
         <v>2.961</v>
       </c>
     </row>
@@ -13235,7 +13234,7 @@
       <c r="B11" s="8" t="n">
         <v>51.6</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="8" t="n">
         <v>2.974</v>
       </c>
     </row>
@@ -13246,7 +13245,7 @@
       <c r="B12" s="8" t="n">
         <v>56.66</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="8" t="n">
         <v>2.752</v>
       </c>
     </row>
@@ -13257,7 +13256,7 @@
       <c r="B13" s="8" t="n">
         <v>57.95</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="8" t="n">
         <v>3.074</v>
       </c>
     </row>
@@ -13268,7 +13267,7 @@
       <c r="B14" s="8" t="n">
         <v>63.66</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="8" t="n">
         <v>2.738</v>
       </c>
     </row>
@@ -13279,7 +13278,7 @@
       <c r="B15" s="8" t="n">
         <v>62.18</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="8" t="n">
         <v>3.631</v>
       </c>
     </row>
@@ -13290,7 +13289,7 @@
       <c r="B16" s="8" t="n">
         <v>62.77</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="8" t="n">
         <v>2.639</v>
       </c>
     </row>
@@ -13301,7 +13300,7 @@
       <c r="B17" s="8" t="n">
         <v>66.33</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="8" t="n">
         <v>2.691</v>
       </c>
     </row>
@@ -13312,7 +13311,7 @@
       <c r="B18" s="8" t="n">
         <v>69.98</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="8" t="n">
         <v>2.821</v>
       </c>
     </row>
@@ -13323,7 +13322,7 @@
       <c r="B19" s="8" t="n">
         <v>67.31999999999999</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="8" t="n">
         <v>2.875</v>
       </c>
     </row>
@@ -13334,7 +13333,7 @@
       <c r="B20" s="8" t="n">
         <v>70.58</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" s="8" t="n">
         <v>2.996</v>
       </c>
     </row>
@@ -13345,7 +13344,7 @@
       <c r="B21" s="8" t="n">
         <v>67.84999999999999</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" s="8" t="n">
         <v>2.822</v>
       </c>
     </row>
@@ -13356,7 +13355,7 @@
       <c r="B22" s="8" t="n">
         <v>70.09</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" s="8" t="n">
         <v>2.895</v>
       </c>
     </row>
@@ -13367,7 +13366,7 @@
       <c r="B23" s="8" t="n">
         <v>70.76000000000001</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" s="8" t="n">
         <v>3.021</v>
       </c>
     </row>
@@ -13378,7 +13377,7 @@
       <c r="B24" s="8" t="n">
         <v>56.69</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" s="8" t="n">
         <v>3.185</v>
       </c>
     </row>
@@ -13389,7 +13388,7 @@
       <c r="B25" s="8" t="n">
         <v>48.98</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="8" t="n">
         <v>4.715</v>
       </c>
     </row>
@@ -13400,7 +13399,7 @@
       <c r="B26" s="8" t="n">
         <v>51.55</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="8" t="n">
         <v>3.642</v>
       </c>
     </row>
@@ -13411,7 +13410,7 @@
       <c r="B27" s="8" t="n">
         <v>54.98</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" s="8" t="n">
         <v>2.95</v>
       </c>
     </row>
@@ -13422,7 +13421,7 @@
       <c r="B28" s="8" t="n">
         <v>58.17</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="8" t="n">
         <v>2.855</v>
       </c>
     </row>
@@ -13433,7 +13432,7 @@
       <c r="B29" s="8" t="n">
         <v>63.87</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" s="8" t="n">
         <v>2.713</v>
       </c>
     </row>
@@ -13444,7 +13443,7 @@
       <c r="B30" s="8" t="n">
         <v>60.87</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" s="8" t="n">
         <v>2.566</v>
       </c>
     </row>
@@ -13455,7 +13454,7 @@
       <c r="B31" s="8" t="n">
         <v>54.71</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" s="8" t="n">
         <v>2.633</v>
       </c>
     </row>
@@ -13466,7 +13465,7 @@
       <c r="B32" s="8" t="n">
         <v>57.55</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" s="8" t="n">
         <v>2.291</v>
       </c>
     </row>
@@ -13477,7 +13476,7 @@
       <c r="B33" s="8" t="n">
         <v>54.84</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" s="8" t="n">
         <v>2.141</v>
       </c>
     </row>
@@ -13488,7 +13487,7 @@
       <c r="B34" s="8" t="n">
         <v>56.97</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" s="8" t="n">
         <v>2.251</v>
       </c>
     </row>
@@ -13499,7 +13498,7 @@
       <c r="B35" s="8" t="n">
         <v>54.01</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" s="8" t="n">
         <v>2.428</v>
       </c>
     </row>
@@ -13510,7 +13509,7 @@
       <c r="B36" s="8" t="n">
         <v>57.07</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" s="8" t="n">
         <v>2.597</v>
       </c>
     </row>
@@ -13521,7 +13520,7 @@
       <c r="B37" s="8" t="n">
         <v>59.81</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" s="8" t="n">
         <v>2.47</v>
       </c>
     </row>
@@ -13532,7 +13531,7 @@
       <c r="B38" s="8" t="n">
         <v>57.53</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" s="8" t="n">
         <v>2.158</v>
       </c>
     </row>
@@ -13543,7 +13542,7 @@
       <c r="B39" s="8" t="n">
         <v>50.54</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" s="8" t="n">
         <v>1.877</v>
       </c>
     </row>
@@ -13554,7 +13553,7 @@
       <c r="B40" s="8" t="n">
         <v>30.45</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" s="8" t="n">
         <v>1.821</v>
       </c>
     </row>
@@ -13565,7 +13564,7 @@
       <c r="B41" s="8" t="n">
         <v>16.7</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" s="8" t="n">
         <v>1.634</v>
       </c>
     </row>
@@ -13576,7 +13575,7 @@
       <c r="B42" s="8" t="n">
         <v>28.53</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" s="8" t="n">
         <v>1.794</v>
       </c>
     </row>
@@ -13587,7 +13586,7 @@
       <c r="B43" s="8" t="n">
         <v>38.31</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" s="8" t="n">
         <v>1.722</v>
       </c>
     </row>
@@ -13598,7 +13597,7 @@
       <c r="B44" s="8" t="n">
         <v>40.77</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" s="8" t="n">
         <v>1.495</v>
       </c>
     </row>
@@ -13609,7 +13608,7 @@
       <c r="B45" s="8" t="n">
         <v>42.39</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" s="8" t="n">
         <v>1.854</v>
       </c>
     </row>
@@ -13620,7 +13619,7 @@
       <c r="B46" s="8" t="n">
         <v>39.63</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" s="8" t="n">
         <v>2.579</v>
       </c>
     </row>
@@ -13631,7 +13630,7 @@
       <c r="B47" s="8" t="n">
         <v>39.56</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" s="8" t="n">
         <v>2.101</v>
       </c>
     </row>
@@ -13642,7 +13641,7 @@
       <c r="B48" s="8" t="n">
         <v>41.35</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48" s="8" t="n">
         <v>2.996</v>
       </c>
     </row>
@@ -13653,7 +13652,7 @@
       <c r="B49" s="8" t="n">
         <v>47.07</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49" s="8" t="n">
         <v>2.896</v>
       </c>
     </row>
@@ -13664,7 +13663,7 @@
       <c r="B50" s="8" t="n">
         <v>52.1</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" s="8" t="n">
         <v>2.467</v>
       </c>
     </row>
@@ -13675,7 +13674,7 @@
       <c r="B51" s="8" t="n">
         <v>59.06</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51" s="8" t="n">
         <v>2.76</v>
       </c>
     </row>
@@ -13686,7 +13685,7 @@
       <c r="B52" s="8" t="n">
         <v>62.36</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52" s="8" t="n">
         <v>2.854</v>
       </c>
     </row>
@@ -13697,7 +13696,7 @@
       <c r="B53" s="8" t="n">
         <v>61.7</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53" s="8" t="n">
         <v>2.586</v>
       </c>
     </row>
@@ -13708,7 +13707,7 @@
       <c r="B54" s="8" t="n">
         <v>65.16</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" s="8" t="n">
         <v>2.925</v>
       </c>
     </row>
@@ -13719,7 +13718,7 @@
       <c r="B55" s="8" t="n">
         <v>71.34999999999999</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" s="8" t="n">
         <v>2.984</v>
       </c>
     </row>
@@ -13730,7 +13729,7 @@
       <c r="B56" s="8" t="n">
         <v>72.43000000000001</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56" s="8" t="n">
         <v>3.617</v>
       </c>
     </row>
@@ -13741,7 +13740,7 @@
       <c r="B57" s="8" t="n">
         <v>67.70999999999999</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57" s="8" t="n">
         <v>4.044</v>
       </c>
     </row>
@@ -13752,7 +13751,7 @@
       <c r="B58" s="8" t="n">
         <v>71.55</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58" s="8" t="n">
         <v>4.37</v>
       </c>
     </row>
@@ -13763,7 +13762,7 @@
       <c r="B59" s="8" t="n">
         <v>81.22</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59" s="8" t="n">
         <v>5.841</v>
       </c>
     </row>
@@ -13774,7 +13773,7 @@
       <c r="B60" s="8" t="n">
         <v>78.65000000000001</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60" s="8" t="n">
         <v>6.202</v>
       </c>
     </row>
@@ -13785,7 +13784,7 @@
       <c r="B61" s="8" t="n">
         <v>71.69</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" s="8" t="n">
         <v>5.447</v>
       </c>
     </row>
@@ -13796,7 +13795,7 @@
       <c r="B62" s="8" t="n">
         <v>82.98</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62" s="8" t="n">
         <v>4.024</v>
       </c>
     </row>
@@ -13807,7 +13806,7 @@
       <c r="B63" s="8" t="n">
         <v>91.63</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63" s="8" t="n">
         <v>6.265</v>
       </c>
     </row>
@@ -13818,7 +13817,7 @@
       <c r="B64" s="8" t="n">
         <v>108.26</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64" s="8" t="n">
         <v>4.568</v>
       </c>
     </row>
@@ -13829,7 +13828,7 @@
       <c r="B65" s="8" t="n">
         <v>101.64</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65" s="8" t="n">
         <v>5.336</v>
       </c>
     </row>
@@ -13840,7 +13839,7 @@
       <c r="B66" s="8" t="n">
         <v>109.26</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66" s="8" t="n">
         <v>7.267</v>
       </c>
     </row>
@@ -13851,7 +13850,7 @@
       <c r="B67" s="8" t="n">
         <v>114.34</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67" s="8" t="n">
         <v>8.907999999999999</v>
       </c>
     </row>
@@ -13862,7 +13861,7 @@
       <c r="B68" s="8" t="n">
         <v>99.39</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68" s="8" t="n">
         <v>6.551</v>
       </c>
     </row>
@@ -13873,7 +13872,7 @@
       <c r="B69" s="8" t="n">
         <v>91.48</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69" s="8" t="n">
         <v>8.686999999999999</v>
       </c>
     </row>
@@ -13884,7 +13883,7 @@
       <c r="B70" s="8" t="n">
         <v>83.8</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70" s="8" t="n">
         <v>9.353</v>
       </c>
     </row>
@@ -13895,7 +13894,7 @@
       <c r="B71" s="8" t="n">
         <v>87.03</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71" s="8" t="n">
         <v>6.868</v>
       </c>
     </row>
@@ -13906,7 +13905,7 @@
       <c r="B72" s="8" t="n">
         <v>84.39</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72" s="8" t="n">
         <v>5.186</v>
       </c>
     </row>
@@ -13917,7 +13916,7 @@
       <c r="B73" s="8" t="n">
         <v>76.52</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73" s="8" t="n">
         <v>6.712</v>
       </c>
     </row>
@@ -13928,7 +13927,7 @@
       <c r="B74" s="8" t="n">
         <v>78.16</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74" s="8" t="n">
         <v>4.709</v>
       </c>
     </row>
@@ -13939,7 +13938,7 @@
       <c r="B75" s="8" t="n">
         <v>76.86</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75" s="8" t="n">
         <v>3.109</v>
       </c>
     </row>
@@ -13950,7 +13949,7 @@
       <c r="B76" s="8" t="n">
         <v>73.37</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76" s="8" t="n">
         <v>2.451</v>
       </c>
     </row>
@@ -13961,7 +13960,7 @@
       <c r="B77" s="8" t="n">
         <v>79.44</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77" s="8" t="n">
         <v>1.991</v>
       </c>
     </row>
@@ -13972,7 +13971,7 @@
       <c r="B78" s="8" t="n">
         <v>71.62</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78" s="8" t="n">
         <v>2.117</v>
       </c>
     </row>
@@ -13983,7 +13982,7 @@
       <c r="B79" s="8" t="n">
         <v>70.27</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79" s="8" t="n">
         <v>2.181</v>
       </c>
     </row>
@@ -13994,7 +13993,7 @@
       <c r="B80" s="8" t="n">
         <v>76.04000000000001</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80" s="8" t="n">
         <v>2.603</v>
       </c>
     </row>
@@ -14005,7 +14004,7 @@
       <c r="B81" s="8" t="n">
         <v>81.31999999999999</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81" s="8" t="n">
         <v>2.492</v>
       </c>
     </row>
@@ -14016,7 +14015,7 @@
       <c r="B82" s="8" t="n">
         <v>89.43000000000001</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82" s="8" t="n">
         <v>2.556</v>
       </c>
     </row>
@@ -14027,7 +14026,7 @@
       <c r="B83" s="8" t="n">
         <v>85.47</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83" s="8" t="n">
         <v>2.764</v>
       </c>
     </row>
@@ -14038,7 +14037,7 @@
       <c r="B84" s="8" t="n">
         <v>77.38</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84" s="8" t="n">
         <v>3.164</v>
       </c>
     </row>
@@ -14049,7 +14048,7 @@
       <c r="B85" s="8" t="n">
         <v>72.12</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85" s="8" t="n">
         <v>2.706</v>
       </c>
     </row>
@@ -14060,7 +14059,7 @@
       <c r="B86" s="8" t="n">
         <v>73.86</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86" s="8" t="n">
         <v>2.619</v>
       </c>
     </row>
@@ -14071,7 +14070,7 @@
       <c r="B87" s="8" t="n">
         <v>76.61</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87" s="8" t="n">
         <v>2.49</v>
       </c>
     </row>
@@ -14082,7 +14081,7 @@
       <c r="B88" s="8" t="n">
         <v>80.41</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88" s="8" t="n">
         <v>1.615</v>
       </c>
     </row>
@@ -14093,18 +14092,18 @@
       <c r="B89" s="8" t="n">
         <v>84.39</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89" s="8" t="n">
         <v>1.575</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="9" t="n">
+      <c r="A90" s="7" t="n">
         <v>45413</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90" s="8" t="n">
         <v>78.62</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90" s="8" t="n">
         <v>1.614</v>
       </c>
     </row>

</xml_diff>